<commit_message>
setup gui with tkinter
</commit_message>
<xml_diff>
--- a/results/compatibility.xlsx
+++ b/results/compatibility.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Make</t>
   </si>
@@ -34,64 +34,49 @@
     <t>VOLVO</t>
   </si>
   <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>2022-2023</t>
-  </si>
-  <si>
-    <t>Rear or Front</t>
-  </si>
-  <si>
     <t>S60</t>
   </si>
   <si>
-    <t>2019-2023</t>
-  </si>
-  <si>
-    <t>AWD</t>
+    <t>2019-2020</t>
+  </si>
+  <si>
+    <t>Front</t>
   </si>
   <si>
     <t>S90</t>
   </si>
   <si>
-    <t>2017-2023</t>
+    <t>2017-2019</t>
   </si>
   <si>
     <t>V60</t>
   </si>
   <si>
+    <t>No 2.0L L4 ELECTRIC/GAS Turbocharged</t>
+  </si>
+  <si>
     <t>V90</t>
   </si>
   <si>
-    <t>2018-2023</t>
+    <t>2018-2019</t>
   </si>
   <si>
     <t>V90 CROSS COUNTRY</t>
   </si>
   <si>
-    <t>2017-2021</t>
-  </si>
-  <si>
-    <t>XC40</t>
-  </si>
-  <si>
-    <t>2021-2023</t>
-  </si>
-  <si>
-    <t>No 2.0L L4 Turbocharged</t>
+    <t>2017</t>
   </si>
   <si>
     <t>XC60</t>
   </si>
   <si>
+    <t>2018-2020</t>
+  </si>
+  <si>
     <t>XC90</t>
   </si>
   <si>
-    <t>2016-2023</t>
-  </si>
-  <si>
-    <t>B5 Core or B6 Core or B6 Plus or B6 Ultimate</t>
+    <t>2016-2019</t>
   </si>
 </sst>
 </file>
@@ -466,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,38 +505,34 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="20.25" customHeight="1">
@@ -597,43 +578,7 @@
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more ai things
</commit_message>
<xml_diff>
--- a/results/compatibility.xlsx
+++ b/results/compatibility.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Make</t>
   </si>
@@ -34,49 +34,64 @@
     <t>VOLVO</t>
   </si>
   <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Rear or Front</t>
+  </si>
+  <si>
     <t>S60</t>
   </si>
   <si>
-    <t>2019-2020</t>
-  </si>
-  <si>
-    <t>Front</t>
+    <t>2019-2023</t>
+  </si>
+  <si>
+    <t>AWD</t>
   </si>
   <si>
     <t>S90</t>
   </si>
   <si>
-    <t>2017-2019</t>
+    <t>2017-2023</t>
   </si>
   <si>
     <t>V60</t>
   </si>
   <si>
-    <t>No 2.0L L4 ELECTRIC/GAS Turbocharged</t>
-  </si>
-  <si>
     <t>V90</t>
   </si>
   <si>
-    <t>2018-2019</t>
+    <t>2018-2023</t>
   </si>
   <si>
     <t>V90 CROSS COUNTRY</t>
   </si>
   <si>
-    <t>2017</t>
+    <t>2017-2021</t>
+  </si>
+  <si>
+    <t>XC40</t>
+  </si>
+  <si>
+    <t>2021-2023</t>
+  </si>
+  <si>
+    <t>No 2.0L L4 Turbocharged</t>
   </si>
   <si>
     <t>XC60</t>
   </si>
   <si>
-    <t>2018-2020</t>
-  </si>
-  <si>
     <t>XC90</t>
   </si>
   <si>
-    <t>2016-2019</t>
+    <t>2016-2023</t>
+  </si>
+  <si>
+    <t>B5 Core or B6 Core or B6 Plus or B6 Ultimate</t>
   </si>
 </sst>
 </file>
@@ -451,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,34 +520,38 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="20.25" customHeight="1">
@@ -578,7 +597,43 @@
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>